<commit_message>
ignore updates and more case details
</commit_message>
<xml_diff>
--- a/assets/slides/acct3210/S7/case.xlsx
+++ b/assets/slides/acct3210/S7/case.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ACCT3210_materials/slides/S7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ArthurHowardMorris.github.io/assets/slides/acct3210/S7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A9F119-C078-F248-A5BB-73FCC1C36290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AF09AD-6F49-3848-A954-2A4FD5F3DD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42360" yWindow="21080" windowWidth="26840" windowHeight="15940" activeTab="2" xr2:uid="{C00C2333-4917-5D42-BB89-93715C7EFC19}"/>
+    <workbookView xWindow="9080" yWindow="4380" windowWidth="26840" windowHeight="15940" xr2:uid="{C00C2333-4917-5D42-BB89-93715C7EFC19}"/>
   </bookViews>
   <sheets>
-    <sheet name="simple" sheetId="3" r:id="rId1"/>
-    <sheet name="what matters" sheetId="1" r:id="rId2"/>
-    <sheet name="npv" sheetId="2" r:id="rId3"/>
+    <sheet name="contents" sheetId="5" r:id="rId1"/>
+    <sheet name="simple" sheetId="3" r:id="rId2"/>
+    <sheet name="what matters" sheetId="1" r:id="rId3"/>
+    <sheet name="npv v1" sheetId="2" r:id="rId4"/>
+    <sheet name="npv v2" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,8 +75,44 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B781F698-F9D3-6743-9665-8876523E404D}</author>
+    <author>tc={7BB4F94D-373F-CF4C-8E97-AA865D4B717F}</author>
+    <author>tc={31E66A97-8F8A-374D-B6C3-0540E7C4309B}</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{B781F698-F9D3-6743-9665-8876523E404D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I’m calling this 2022, but think of this as “now” or more specifically the beginning of 2023</t>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="1" shapeId="0" xr:uid="{7BB4F94D-373F-CF4C-8E97-AA865D4B717F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We don’t include the cost of operations for 2023 because we incur them in both scenarios.</t>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="2" shapeId="0" xr:uid="{31E66A97-8F8A-374D-B6C3-0540E7C4309B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is the 89,000 we pay the new manager minus the 10,000 that we do not have to give the old manager for the new job. This bonus could get it’s own line below.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="74">
   <si>
     <t>New Machine:</t>
   </si>
@@ -263,6 +301,39 @@
   </si>
   <si>
     <t>Investment</t>
+  </si>
+  <si>
+    <t>This is a page of free form notes to give some context about my workflow.</t>
+  </si>
+  <si>
+    <t>raise for old manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet name </t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>a simple example of calculating the NPV of a series of cash flows</t>
+  </si>
+  <si>
+    <t>what matters</t>
+  </si>
+  <si>
+    <t>a sheet with free form notes where I start to gather the bits of information that I will use</t>
+  </si>
+  <si>
+    <t>npv v1</t>
+  </si>
+  <si>
+    <t>this is my preferred method for setting up the problem</t>
+  </si>
+  <si>
+    <t>npv v2</t>
+  </si>
+  <si>
+    <t>this is an equally valid approach which attemps to be more explicit</t>
   </si>
 </sst>
 </file>
@@ -272,9 +343,9 @@
   <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -354,6 +425,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -423,7 +501,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -444,12 +522,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -784,7 +864,76 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B3" dT="2023-02-27T23:33:35.63" personId="{1C1CB457-E2F2-B648-84DE-1AA844AD795C}" id="{B781F698-F9D3-6743-9665-8876523E404D}">
+    <text>I’m calling this 2022, but think of this as “now” or more specifically the beginning of 2023</text>
+  </threadedComment>
+  <threadedComment ref="C6" dT="2023-02-28T10:21:52.42" personId="{1C1CB457-E2F2-B648-84DE-1AA844AD795C}" id="{7BB4F94D-373F-CF4C-8E97-AA865D4B717F}">
+    <text>We don’t include the cost of operations for 2023 because we incur them in both scenarios.</text>
+  </threadedComment>
+  <threadedComment ref="C7" dT="2023-02-28T10:24:15.45" personId="{1C1CB457-E2F2-B648-84DE-1AA844AD795C}" id="{31E66A97-8F8A-374D-B6C3-0540E7C4309B}">
+    <text>This is the 89,000 we pay the new manager minus the 10,000 that we do not have to give the old manager for the new job. This bonus could get it’s own line below.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EF05B2-74A1-D14F-857C-FC650027815B}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4645617-069A-0F46-A953-9B9A846127BD}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -921,12 +1070,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F12574F-0551-3041-9840-066F27AE6BF7}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,344 +1085,349 @@
     <col min="3" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
+    <row r="1" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1100000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1700000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
+      <c r="F3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1100000</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>1700000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>4000</v>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>4000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <f>6500*50</f>
         <v>325000</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <f>6500*80</f>
         <v>520000</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>40000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>20000</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>40000</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17">
         <f>75000+89000</f>
         <v>164000</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>85000</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="D17">
+        <f>B17-C17</f>
         <v>79000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="10">
-        <v>2000</v>
-      </c>
-      <c r="C19" s="10">
-        <v>2000</v>
-      </c>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="10">
-        <v>2000</v>
-      </c>
-      <c r="C20" s="10">
-        <v>500</v>
-      </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="11">
-        <v>3750000</v>
-      </c>
-      <c r="C21" s="11">
-        <v>1000000</v>
-      </c>
-      <c r="D21" s="11">
-        <v>4750000</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B21" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2000</v>
+      </c>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="11">
-        <v>2600000</v>
-      </c>
-      <c r="C22" s="11">
-        <v>400000</v>
-      </c>
-      <c r="D22" s="11">
-        <v>3000000</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B22" s="10">
+        <v>2000</v>
+      </c>
+      <c r="C22" s="10">
+        <v>500</v>
+      </c>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="11">
-        <v>600000</v>
+        <v>3750000</v>
       </c>
       <c r="C23" s="11">
-        <v>150000</v>
+        <v>1000000</v>
       </c>
       <c r="D23" s="11">
-        <v>750000</v>
+        <v>4750000</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="11">
-        <v>3200000</v>
+        <v>2600000</v>
       </c>
       <c r="C24" s="11">
-        <v>550000</v>
+        <v>400000</v>
       </c>
       <c r="D24" s="11">
-        <v>3750000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="11">
+        <v>600000</v>
+      </c>
+      <c r="C25" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D25" s="11">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="11">
+        <v>3200000</v>
+      </c>
+      <c r="C26" s="11">
+        <v>550000</v>
+      </c>
+      <c r="D26" s="11">
+        <v>3750000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11">
         <v>1000000</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9">
-        <v>200000</v>
-      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9">
         <v>75000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="13">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="12">
-        <v>325000</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="6">
-        <v>850000</v>
+      <c r="D32" s="13">
+        <v>100000</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="7">
-        <v>150000</v>
+      <c r="D33" s="12">
+        <v>325000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6">
+        <v>850000</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="7">
+        <v>150000</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1282,11 +1436,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1891ED6A-8201-4441-9DDB-F3B0CCF23FA7}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1479,27 +1633,27 @@
         <v>51</v>
       </c>
       <c r="B10" s="1">
-        <f>SUM(B4:B9)</f>
+        <f t="shared" ref="B10:G10" si="1">SUM(B4:B9)</f>
         <v>-1100000</v>
       </c>
       <c r="C10" s="1">
-        <f>SUM(C4:C9)</f>
+        <f t="shared" si="1"/>
         <v>861000</v>
       </c>
       <c r="D10" s="1">
-        <f>SUM(D4:D9)</f>
+        <f t="shared" si="1"/>
         <v>341000</v>
       </c>
       <c r="E10" s="1">
-        <f>SUM(E4:E9)</f>
+        <f t="shared" si="1"/>
         <v>861000</v>
       </c>
       <c r="F10" s="1">
-        <f>SUM(F4:F9)</f>
+        <f t="shared" si="1"/>
         <v>861000</v>
       </c>
       <c r="G10" s="1">
-        <f>SUM(G4:G9)</f>
+        <f t="shared" si="1"/>
         <v>961000</v>
       </c>
     </row>
@@ -1508,27 +1662,27 @@
         <v>53</v>
       </c>
       <c r="B11" s="15">
-        <f>B3-$B$3</f>
+        <f t="shared" ref="B11:G11" si="2">B3-$B$3</f>
         <v>0</v>
       </c>
       <c r="C11" s="15">
-        <f>C3-$B$3</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D11" s="15">
-        <f>D3-$B$3</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E11" s="15">
-        <f>E3-$B$3</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="F11" s="15">
-        <f>F3-$B$3</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="G11" s="15">
-        <f>G3-$B$3</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -1537,27 +1691,27 @@
         <v>54</v>
       </c>
       <c r="B12" s="1">
-        <f>(B10)/((1+$B$1)^B11)</f>
+        <f t="shared" ref="B12:G12" si="3">(B10)/((1+$B$1)^B11)</f>
         <v>-1100000</v>
       </c>
       <c r="C12" s="1">
-        <f>(C10)/((1+$B$1)^C11)</f>
+        <f t="shared" si="3"/>
         <v>782727.27272727271</v>
       </c>
       <c r="D12" s="1">
-        <f>(D10)/((1+$B$1)^D11)</f>
+        <f t="shared" si="3"/>
         <v>281818.18181818177</v>
       </c>
       <c r="E12" s="1">
-        <f>(E10)/((1+$B$1)^E11)</f>
+        <f t="shared" si="3"/>
         <v>646882.04357625823</v>
       </c>
       <c r="F12" s="1">
-        <f>(F10)/((1+$B$1)^F11)</f>
+        <f t="shared" si="3"/>
         <v>588074.58506932575</v>
       </c>
       <c r="G12" s="1">
-        <f>(G10)/((1+$B$1)^G11)</f>
+        <f t="shared" si="3"/>
         <v>596705.39145984792</v>
       </c>
     </row>
@@ -1594,6 +1748,428 @@
       </c>
       <c r="B16" s="1">
         <v>1700000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513AF158-0DB5-5843-9E42-5F724975E01F}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>2022</v>
+      </c>
+      <c r="C3">
+        <v>2023</v>
+      </c>
+      <c r="D3">
+        <v>2024</v>
+      </c>
+      <c r="E3">
+        <v>2025</v>
+      </c>
+      <c r="F3">
+        <v>2026</v>
+      </c>
+      <c r="G3">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1000000</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-60000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-60000</v>
+      </c>
+      <c r="E5" s="14">
+        <v>-60000</v>
+      </c>
+      <c r="F5" s="14">
+        <v>-60000</v>
+      </c>
+      <c r="G5" s="14">
+        <v>-60000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f>-6500*80</f>
+        <v>-520000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f>-89000</f>
+        <v>-89000</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:G7" si="0">-89000</f>
+        <v>-89000</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>-89000</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>-89000</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>-89000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-1100000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ref="B10:G10" si="1">SUM(B4:B9)</f>
+        <v>-1100000</v>
+      </c>
+      <c r="C10" s="1">
+        <f>SUM(C4:C9)</f>
+        <v>851000</v>
+      </c>
+      <c r="D10" s="1">
+        <f>SUM(D4:D9)</f>
+        <v>331000</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUM(E4:E9)</f>
+        <v>851000</v>
+      </c>
+      <c r="F10" s="1">
+        <f>SUM(F4:F9)</f>
+        <v>851000</v>
+      </c>
+      <c r="G10" s="1">
+        <f>SUM(G4:G9)</f>
+        <v>951000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="15">
+        <f t="shared" ref="B11:G11" si="2">B3-$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="F11" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G11" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" ref="B12:G12" si="3">(B10)/((1+$B$1)^B11)</f>
+        <v>-1100000</v>
+      </c>
+      <c r="C12" s="1">
+        <f>(C10)/((1+$B$1)^C11)</f>
+        <v>773636.36363636353</v>
+      </c>
+      <c r="D12" s="1">
+        <f>(D10)/((1+$B$1)^D11)</f>
+        <v>273553.71900826442</v>
+      </c>
+      <c r="E12" s="1">
+        <f>(E10)/((1+$B$1)^E11)</f>
+        <v>639368.89556724252</v>
+      </c>
+      <c r="F12" s="1">
+        <f>(F10)/((1+$B$1)^F11)</f>
+        <v>581244.45051567501</v>
+      </c>
+      <c r="G12" s="1">
+        <f>(G10)/((1+$B$1)^G11)</f>
+        <v>590496.17822925642</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="22">
+        <f>SUM(B12:G12)</f>
+        <v>1758299.6069568018</v>
+      </c>
+      <c r="C13" s="23">
+        <f>NPV(B1,C10:G10)+B9</f>
+        <v>1758299.6069568023</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>2022</v>
+      </c>
+      <c r="C15">
+        <v>2023</v>
+      </c>
+      <c r="D15">
+        <v>2024</v>
+      </c>
+      <c r="E15">
+        <v>2025</v>
+      </c>
+      <c r="F15">
+        <v>2026</v>
+      </c>
+      <c r="G15">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17">
+        <v>-10000</v>
+      </c>
+      <c r="D17">
+        <v>-10000</v>
+      </c>
+      <c r="E17">
+        <v>-10000</v>
+      </c>
+      <c r="F17">
+        <v>-10000</v>
+      </c>
+      <c r="G17">
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="25">
+        <f>SUM(B16:B17)</f>
+        <v>1700000</v>
+      </c>
+      <c r="C18" s="25">
+        <f t="shared" ref="C18:G18" si="4">SUM(C16:C17)</f>
+        <v>-10000</v>
+      </c>
+      <c r="D18" s="25">
+        <f t="shared" si="4"/>
+        <v>-10000</v>
+      </c>
+      <c r="E18" s="25">
+        <f t="shared" si="4"/>
+        <v>-10000</v>
+      </c>
+      <c r="F18" s="25">
+        <f t="shared" si="4"/>
+        <v>-10000</v>
+      </c>
+      <c r="G18" s="25">
+        <f t="shared" si="4"/>
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="25">
+        <f>(B18)/((1+$B$1)^B11)</f>
+        <v>1700000</v>
+      </c>
+      <c r="C19" s="25">
+        <f t="shared" ref="C19:G19" si="5">(C18)/((1+$B$1)^C11)</f>
+        <v>-9090.9090909090901</v>
+      </c>
+      <c r="D19" s="25">
+        <f t="shared" si="5"/>
+        <v>-8264.4628099173533</v>
+      </c>
+      <c r="E19" s="25">
+        <f t="shared" si="5"/>
+        <v>-7513.1480090157756</v>
+      </c>
+      <c r="F19" s="25">
+        <f t="shared" si="5"/>
+        <v>-6830.1345536507051</v>
+      </c>
+      <c r="G19" s="25">
+        <f t="shared" si="5"/>
+        <v>-6209.2132305915493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="25">
+        <f>SUM(B19:G19)</f>
+        <v>1662092.1323059157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added details on the example
</commit_message>
<xml_diff>
--- a/assets/slides/acct3210/S7/case.xlsx
+++ b/assets/slides/acct3210/S7/case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shamussiothrun/ArthurHowardMorris.github.io/assets/slides/acct3210/S7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DAE4FD-DE8D-254E-AB33-09A0EE6F32B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7D9D6A-01B0-1D4C-B273-D157F3C21623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9080" yWindow="4380" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{C00C2333-4917-5D42-BB89-93715C7EFC19}"/>
+    <workbookView xWindow="9080" yWindow="4380" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{C00C2333-4917-5D42-BB89-93715C7EFC19}"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="5" r:id="rId1"/>
@@ -345,7 +345,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,12 +418,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -528,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -937,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4645617-069A-0F46-A953-9B9A846127BD}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -979,8 +973,8 @@
         <v>250000</v>
       </c>
       <c r="C4" s="18">
-        <f>B4/((1+$F$2)^A4)</f>
-        <v>250000</v>
+        <f>B4/((1+$B$2)^A4)</f>
+        <v>223214.28571428568</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -991,8 +985,8 @@
         <v>300000</v>
       </c>
       <c r="C5" s="18">
-        <f>B5/((1+$F$2)^A5)</f>
-        <v>300000</v>
+        <f t="shared" ref="C5:C9" si="0">B5/((1+$B$2)^A5)</f>
+        <v>239158.1632653061</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1003,8 +997,8 @@
         <v>340000</v>
       </c>
       <c r="C6" s="18">
-        <f>B6/((1+$F$2)^A6)</f>
-        <v>340000</v>
+        <f t="shared" si="0"/>
+        <v>242005.28425655971</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1015,8 +1009,8 @@
         <v>375000</v>
       </c>
       <c r="C7" s="18">
-        <f>B7/((1+$F$2)^A7)</f>
-        <v>375000</v>
+        <f t="shared" si="0"/>
+        <v>238319.27940181168</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1026,9 +1020,9 @@
       <c r="B8" s="20">
         <v>300000</v>
       </c>
-      <c r="C8" s="18">
-        <f>B8/((1+$F$2)^A8)</f>
-        <v>300000</v>
+      <c r="C8" s="20">
+        <f t="shared" si="0"/>
+        <v>170228.05671557976</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1041,7 +1035,7 @@
       </c>
       <c r="C9" s="18">
         <f>SUM(C4:C8)</f>
-        <v>1565000</v>
+        <v>1112925.069353543</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1760,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513AF158-0DB5-5843-9E42-5F724975E01F}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1953,7 +1947,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ref="B10:G10" si="1">SUM(B4:B9)</f>
+        <f t="shared" ref="B10" si="1">SUM(B4:B9)</f>
         <v>-1100000</v>
       </c>
       <c r="C10" s="1">
@@ -2011,7 +2005,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" ref="B12:G12" si="3">(B10)/((1+$B$1)^B11)</f>
+        <f t="shared" ref="B12" si="3">(B10)/((1+$B$1)^B11)</f>
         <v>-1100000</v>
       </c>
       <c r="C12" s="1">

</xml_diff>